<commit_message>
run S1 no imports exports
</commit_message>
<xml_diff>
--- a/data/MostImportantData.xlsx
+++ b/data/MostImportantData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447A2DE8-1553-4471-A555-8ADE7C9A208C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE893D1-76EE-4D54-90F7-2A91E9250872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="-20370" windowWidth="26130" windowHeight="16590" tabRatio="738" activeTab="1" xr2:uid="{B8782AFC-8070-4987-A54E-8F4783B58729}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="738" activeTab="3" xr2:uid="{B8782AFC-8070-4987-A54E-8F4783B58729}"/>
   </bookViews>
   <sheets>
     <sheet name="Technology" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="216">
   <si>
     <t>ElectricitySportMarket</t>
   </si>
@@ -655,19 +655,67 @@
     <t>MW</t>
   </si>
   <si>
-    <t>lifetime</t>
-  </si>
-  <si>
-    <t>permit time</t>
-  </si>
-  <si>
-    <t>construction time</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
     <t>ENTSOE GA</t>
+  </si>
+  <si>
+    <t>Realistic capacity [MW]</t>
+  </si>
+  <si>
+    <t>permit time [y]</t>
+  </si>
+  <si>
+    <t>construction time [y]</t>
+  </si>
+  <si>
+    <t>lifetime [y]</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Natural gas</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>Investment costs [Eur/MW]</t>
+  </si>
+  <si>
+    <t>Efficiency [%]</t>
+  </si>
+  <si>
+    <t>Fixed costs [Eur/Mwh/year]</t>
+  </si>
+  <si>
+    <t>Variable costs [Eur/MWh]</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>VOLL [Eur/MWh]</t>
+  </si>
+  <si>
+    <t>Industrial</t>
+  </si>
+  <si>
+    <t>Household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrogen </t>
+  </si>
+  <si>
+    <t>Percentage demand</t>
   </si>
 </sst>
 </file>
@@ -883,7 +931,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -941,6 +989,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -995,7 +1056,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1039,6 +1100,9 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="31"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{660B22D1-3511-451A-B770-8E4B2498B7FA}"/>
@@ -4137,13 +4201,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>153707</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>54402</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>578437</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>120798</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4277,9 +4341,6 @@
           <cell r="B1" t="str">
             <v>Technology</v>
           </cell>
-          <cell r="D1" t="str">
-            <v>Realistic_capacity</v>
-          </cell>
         </row>
         <row r="2">
           <cell r="B2" t="str">
@@ -4329,12 +4390,25 @@
             <v>300</v>
           </cell>
         </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>PV_residential</v>
+          </cell>
+          <cell r="D8">
+            <v>300</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Nuclear</v>
+          </cell>
+          <cell r="D9">
+            <v>1000</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="9">
         <row r="1">
-          <cell r="A1" t="str">
-            <v>traderes technology</v>
-          </cell>
           <cell r="B1" t="str">
             <v>type</v>
           </cell>
@@ -4673,47 +4747,47 @@
         </row>
         <row r="18">
           <cell r="A18" t="str">
-            <v>Hydropower_reservoir_medium</v>
+            <v>PV_residential</v>
           </cell>
           <cell r="B18" t="str">
             <v>VariableRenewableOperator</v>
           </cell>
           <cell r="C18">
-            <v>2</v>
+            <v>1</v>
           </cell>
           <cell r="D18">
-            <v>5</v>
+            <v>1</v>
           </cell>
           <cell r="E18">
-            <v>60</v>
+            <v>25</v>
           </cell>
           <cell r="F18">
-            <v>60</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19" t="str">
-            <v>hydrogen_turbine</v>
+            <v>Hydropower_reservoir_medium</v>
           </cell>
           <cell r="B19" t="str">
-            <v>ConventionalPlantOperator</v>
+            <v>VariableRenewableOperator</v>
           </cell>
           <cell r="C19">
             <v>2</v>
           </cell>
           <cell r="D19">
-            <v>2</v>
+            <v>5</v>
           </cell>
           <cell r="E19">
-            <v>30</v>
+            <v>60</v>
           </cell>
           <cell r="F19">
-            <v>30</v>
+            <v>60</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20" t="str">
-            <v>hydrogen_CHP</v>
+            <v>hydrogen_turbine</v>
           </cell>
           <cell r="B20" t="str">
             <v>ConventionalPlantOperator</v>
@@ -4728,26 +4802,6 @@
             <v>30</v>
           </cell>
           <cell r="F20">
-            <v>30</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>hydrogen_combined_cycle</v>
-          </cell>
-          <cell r="B21" t="str">
-            <v>ConventionalPlantOperator</v>
-          </cell>
-          <cell r="C21">
-            <v>2</v>
-          </cell>
-          <cell r="D21">
-            <v>2</v>
-          </cell>
-          <cell r="E21">
-            <v>30</v>
-          </cell>
-          <cell r="F21">
             <v>30</v>
           </cell>
         </row>
@@ -4833,7 +4887,7 @@
         </row>
         <row r="3">
           <cell r="A3" t="str">
-            <v>DutchElectricitySpotMarket</v>
+            <v>ElectricitySpotMarketNL</v>
           </cell>
           <cell r="B3">
             <v>4000</v>
@@ -4846,15 +4900,6 @@
           <cell r="A1" t="str">
             <v>Name</v>
           </cell>
-          <cell r="B1" t="str">
-            <v>VOLL</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>TimeSeriesFile</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>TimeSeriesFileFuture</v>
-          </cell>
         </row>
         <row r="2">
           <cell r="A2" t="str">
@@ -4863,9 +4908,6 @@
           <cell r="B2">
             <v>4000</v>
           </cell>
-          <cell r="C2" t="str">
-            <v>amiris-config/data/load.csv</v>
-          </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
@@ -4874,9 +4916,6 @@
           <cell r="B3">
             <v>1500</v>
           </cell>
-          <cell r="C3" t="str">
-            <v>amiris-config/data/LS_high.csv</v>
-          </cell>
           <cell r="F3">
             <v>0.1</v>
           </cell>
@@ -4888,9 +4927,6 @@
           <cell r="B4">
             <v>500</v>
           </cell>
-          <cell r="C4" t="str">
-            <v>amiris-config/data/LS_mid.csv</v>
-          </cell>
           <cell r="F4">
             <v>0.05</v>
           </cell>
@@ -4902,9 +4938,6 @@
           <cell r="B5">
             <v>250</v>
           </cell>
-          <cell r="C5" t="str">
-            <v>amiris-config/data/LS_low.csv</v>
-          </cell>
           <cell r="F5">
             <v>0.05</v>
           </cell>
@@ -4915,12 +4948,6 @@
           </cell>
           <cell r="B6">
             <v>33.374000000000002</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>amiris-config/data/LS_hydrogen_high.csv</v>
-          </cell>
-          <cell r="D6" t="str">
-            <v>amiris-config/data/LS_hydrogen.csv</v>
           </cell>
         </row>
       </sheetData>
@@ -5883,21 +5910,21 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.90625" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="8" max="8" width="7.81640625" customWidth="1"/>
-    <col min="10" max="10" width="7.453125" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -5910,18 +5937,17 @@
         <f>[1]CandidatePowerPlants!B1</f>
         <v>Technology</v>
       </c>
-      <c r="C2" s="6" t="str">
-        <f>[1]CandidatePowerPlants!D1</f>
-        <v>Realistic_capacity</v>
+      <c r="C2" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -5934,15 +5960,15 @@
         <v>100</v>
       </c>
       <c r="D3" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B3,$B$12:$B$31,0),2)</f>
+        <f t="shared" ref="D3:D4" si="0">INDEX($B$14:$F$33,MATCH(B3,$B$14:$B$33,0),2)</f>
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B3,$B$12:$B$31,0),3)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B3,$B$14:$B$33,0),3)</f>
         <v>1</v>
       </c>
       <c r="F3" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B3,$B$12:$B$31,0),4)</f>
+        <f t="shared" ref="F3:F4" si="1">INDEX($B$14:$F$33,MATCH(B3,$B$14:$B$33,0),4)</f>
         <v>20</v>
       </c>
     </row>
@@ -5956,59 +5982,59 @@
         <v>500</v>
       </c>
       <c r="D4" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B4,$B$12:$B$31,0),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B4,$B$12:$B$31,0),3)</f>
+        <f t="shared" ref="E4" si="2">INDEX($B$14:$F$33,MATCH(B4,$B$14:$B$33,0),3)</f>
         <v>2</v>
       </c>
       <c r="F4" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B4,$B$12:$B$31,0),4)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="B5" s="6" t="str">
-        <f>[1]CandidatePowerPlants!B4</f>
-        <v>hydrogen_turbine</v>
+        <f>[1]CandidatePowerPlants!B5</f>
+        <v>PV_utility_systems</v>
       </c>
       <c r="C5" s="6">
-        <f>[1]CandidatePowerPlants!D4</f>
-        <v>500</v>
+        <f>[1]CandidatePowerPlants!D5</f>
+        <v>350</v>
       </c>
       <c r="D5" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B5,$B$12:$B$31,0),2)</f>
-        <v>2</v>
+        <f>INDEX($B$14:$F$33,MATCH(B5,$B$14:$B$33,0),2)</f>
+        <v>1</v>
       </c>
       <c r="E5" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B5,$B$12:$B$31,0),3)</f>
-        <v>2</v>
+        <f>INDEX($B$14:$F$33,MATCH(B5,$B$14:$B$33,0),3)</f>
+        <v>1</v>
       </c>
       <c r="F5" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B5,$B$12:$B$31,0),4)</f>
-        <v>30</v>
+        <f>INDEX($B$14:$F$33,MATCH(B5,$B$14:$B$33,0),4)</f>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" s="6" t="str">
-        <f>[1]CandidatePowerPlants!B5</f>
-        <v>PV_utility_systems</v>
+        <f>[1]CandidatePowerPlants!B8</f>
+        <v>PV_residential</v>
       </c>
       <c r="C6" s="6">
-        <f>[1]CandidatePowerPlants!D5</f>
-        <v>350</v>
+        <f>[1]CandidatePowerPlants!D8</f>
+        <v>300</v>
       </c>
       <c r="D6" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B6,$B$12:$B$31,0),2)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B6,$B$14:$B$33,0),2)</f>
         <v>1</v>
       </c>
       <c r="E6" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B6,$B$12:$B$31,0),3)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B6,$B$14:$B$33,0),3)</f>
         <v>1</v>
       </c>
       <c r="F6" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B6,$B$12:$B$31,0),4)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B6,$B$14:$B$33,0),4)</f>
         <v>25</v>
       </c>
     </row>
@@ -6022,15 +6048,15 @@
         <v>250</v>
       </c>
       <c r="D7" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B7,$B$12:$B$31,0),2)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B7,$B$14:$B$33,0),2)</f>
         <v>1</v>
       </c>
       <c r="E7" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B7,$B$12:$B$31,0),3)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B7,$B$14:$B$33,0),3)</f>
         <v>1</v>
       </c>
       <c r="F7" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B7,$B$12:$B$31,0),4)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B7,$B$14:$B$33,0),4)</f>
         <v>25</v>
       </c>
     </row>
@@ -6044,767 +6070,741 @@
         <v>300</v>
       </c>
       <c r="D8" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B8,$B$12:$B$31,0),2)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B8,$B$14:$B$33,0),2)</f>
         <v>1</v>
       </c>
       <c r="E8" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B8,$B$12:$B$31,0),3)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B8,$B$14:$B$33,0),3)</f>
         <v>3</v>
       </c>
       <c r="F8" s="6">
-        <f>INDEX($B$12:$F$31,MATCH(B8,$B$12:$B$31,0),4)</f>
+        <f>INDEX($B$14:$F$33,MATCH(B8,$B$14:$B$33,0),4)</f>
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="J9" s="5"/>
+      <c r="B9" s="6" t="str">
+        <f>[1]CandidatePowerPlants!B4</f>
+        <v>hydrogen_turbine</v>
+      </c>
+      <c r="C9" s="6">
+        <f>[1]CandidatePowerPlants!D4</f>
+        <v>500</v>
+      </c>
+      <c r="D9" s="6">
+        <f>INDEX($B$14:$F$33,MATCH(B9,$B$14:$B$33,0),2)</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <f>INDEX($B$14:$F$33,MATCH(B9,$B$14:$B$33,0),3)</f>
+        <v>2</v>
+      </c>
+      <c r="F9" s="6">
+        <f>INDEX($B$14:$F$33,MATCH(B9,$B$14:$B$33,0),4)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s">
+      <c r="B10" s="6" t="str">
+        <f>[1]CandidatePowerPlants!B9</f>
+        <v>Nuclear</v>
+      </c>
+      <c r="C10" s="6">
+        <f>[1]CandidatePowerPlants!D9</f>
+        <v>1000</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" ref="D10" si="3">INDEX($B$14:$F$33,MATCH(B10,$B$14:$B$33,0),2)</f>
         <v>2</v>
       </c>
+      <c r="E10" s="6">
+        <f t="shared" ref="E10" si="4">INDEX($B$14:$F$33,MATCH(B10,$B$14:$B$33,0),3)</f>
+        <v>5</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" ref="F10" si="5">INDEX($B$14:$F$33,MATCH(B10,$B$14:$B$33,0),4)</f>
+        <v>45</v>
+      </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="C11" t="str">
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="C13" t="str">
         <f>[1]TechnologiesEmlab!C1</f>
         <v>expectedPermittime</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D13" t="str">
         <f>[1]TechnologiesEmlab!D1</f>
         <v>expectedLeadtime</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E13" t="str">
         <f>[1]TechnologiesEmlab!E1</f>
         <v>lifetime_economic</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F13" t="str">
         <f>[1]TechnologiesEmlab!F1</f>
         <v>lifetime_technical</v>
       </c>
-      <c r="I11" t="str">
+      <c r="I13" t="str">
         <f>[1]TechnologiesEmlab!B1</f>
         <v>type</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="B12" t="str">
+    <row r="14" spans="1:10">
+      <c r="B14" t="str">
         <f>[1]TechnologiesEmlab!A2</f>
         <v>Biomass_CHP_wood_pellets_DH</v>
       </c>
-      <c r="C12">
+      <c r="C14">
         <f>[1]TechnologiesEmlab!C2</f>
         <v>1</v>
       </c>
-      <c r="D12">
+      <c r="D14">
         <f>[1]TechnologiesEmlab!D2</f>
         <v>3</v>
       </c>
-      <c r="E12">
+      <c r="E14">
         <f>[1]TechnologiesEmlab!E2</f>
         <v>30</v>
       </c>
-      <c r="F12">
+      <c r="F14">
         <f>[1]TechnologiesEmlab!F2</f>
         <v>30</v>
       </c>
-      <c r="I12" t="str">
+      <c r="I14" t="str">
         <f>[1]TechnologiesEmlab!B2</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="B13" t="str">
+    <row r="15" spans="1:10">
+      <c r="B15" t="str">
         <f>[1]TechnologiesEmlab!A3</f>
         <v>Biomass_CHP_wood_pellets_PH</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <f>[1]TechnologiesEmlab!C3</f>
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D15">
         <f>[1]TechnologiesEmlab!D3</f>
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <f>[1]TechnologiesEmlab!E3</f>
         <v>20</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <f>[1]TechnologiesEmlab!F3</f>
         <v>20</v>
       </c>
-      <c r="I13" t="str">
+      <c r="I15" t="str">
         <f>[1]TechnologiesEmlab!B3</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="B14" t="str">
+    <row r="16" spans="1:10">
+      <c r="B16" t="str">
         <f>[1]TechnologiesEmlab!A4</f>
         <v>CCGT</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <f>[1]TechnologiesEmlab!C4</f>
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <f>[1]TechnologiesEmlab!D4</f>
         <v>2</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <f>[1]TechnologiesEmlab!E4</f>
         <v>30</v>
       </c>
-      <c r="F14">
+      <c r="F16">
         <f>[1]TechnologiesEmlab!F4</f>
         <v>30</v>
       </c>
-      <c r="I14" t="str">
+      <c r="I16" t="str">
         <f>[1]TechnologiesEmlab!B4</f>
         <v>ConventionalPlantOperator</v>
       </c>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="B15" t="str">
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" t="str">
         <f>[1]TechnologiesEmlab!A5</f>
         <v>CCGT_CHP_backpressure_DH</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <f>[1]TechnologiesEmlab!C5</f>
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <f>[1]TechnologiesEmlab!D5</f>
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <f>[1]TechnologiesEmlab!E5</f>
         <v>30</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <f>[1]TechnologiesEmlab!F5</f>
         <v>30</v>
       </c>
-      <c r="I15" t="str">
+      <c r="I17" t="str">
         <f>[1]TechnologiesEmlab!B5</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="B16" t="str">
+    <row r="18" spans="2:9">
+      <c r="B18" t="str">
         <f>[1]TechnologiesEmlab!A6</f>
         <v>CCGT_CHP_backpressure_PH</v>
       </c>
-      <c r="C16">
+      <c r="C18">
         <f>[1]TechnologiesEmlab!C6</f>
         <v>1</v>
       </c>
-      <c r="D16">
+      <c r="D18">
         <f>[1]TechnologiesEmlab!D6</f>
         <v>2</v>
       </c>
-      <c r="E16">
+      <c r="E18">
         <f>[1]TechnologiesEmlab!E6</f>
         <v>20</v>
       </c>
-      <c r="F16">
+      <c r="F18">
         <f>[1]TechnologiesEmlab!F6</f>
         <v>20</v>
       </c>
-      <c r="I16" t="str">
+      <c r="I18" t="str">
         <f>[1]TechnologiesEmlab!B6</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
-      <c r="B17" t="str">
+    <row r="19" spans="2:9">
+      <c r="B19" t="str">
         <f>[1]TechnologiesEmlab!A7</f>
         <v>CCS</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <f>[1]TechnologiesEmlab!C7</f>
         <v>1</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <f>[1]TechnologiesEmlab!D7</f>
         <v>2</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <f>[1]TechnologiesEmlab!E7</f>
         <v>20</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <f>[1]TechnologiesEmlab!F7</f>
         <v>20</v>
       </c>
-      <c r="I17" t="str">
+      <c r="I19" t="str">
         <f>[1]TechnologiesEmlab!B7</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
-      <c r="B18" t="str">
+    <row r="20" spans="2:9">
+      <c r="B20" t="str">
         <f>[1]TechnologiesEmlab!A8</f>
         <v>Nuclear</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <f>[1]TechnologiesEmlab!C8</f>
         <v>2</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <f>[1]TechnologiesEmlab!D8</f>
         <v>5</v>
       </c>
-      <c r="E18">
+      <c r="E20">
         <f>[1]TechnologiesEmlab!E8</f>
         <v>45</v>
       </c>
-      <c r="F18">
+      <c r="F20">
         <f>[1]TechnologiesEmlab!F8</f>
         <v>45</v>
       </c>
-      <c r="I18" t="str">
+      <c r="I20" t="str">
         <f>[1]TechnologiesEmlab!B8</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
-      <c r="B19" t="str">
+    <row r="21" spans="2:9">
+      <c r="B21" t="str">
         <f>[1]TechnologiesEmlab!A9</f>
         <v>OCGT</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <f>[1]TechnologiesEmlab!C9</f>
         <v>1</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <f>[1]TechnologiesEmlab!D9</f>
         <v>2</v>
       </c>
-      <c r="E19">
+      <c r="E21">
         <f>[1]TechnologiesEmlab!E9</f>
         <v>30</v>
       </c>
-      <c r="F19">
+      <c r="F21">
         <f>[1]TechnologiesEmlab!F9</f>
         <v>30</v>
       </c>
-      <c r="I19" t="str">
+      <c r="I21" t="str">
         <f>[1]TechnologiesEmlab!B9</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
-      <c r="B20" t="str">
+    <row r="22" spans="2:9">
+      <c r="B22" t="str">
         <f>[1]TechnologiesEmlab!A10</f>
         <v>Coal PSC</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <f>[1]TechnologiesEmlab!C10</f>
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D22">
         <f>[1]TechnologiesEmlab!D10</f>
         <v>4</v>
       </c>
-      <c r="E20">
+      <c r="E22">
         <f>[1]TechnologiesEmlab!E10</f>
         <v>40</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <f>[1]TechnologiesEmlab!F10</f>
         <v>40</v>
       </c>
-      <c r="I20" t="str">
+      <c r="I22" t="str">
         <f>[1]TechnologiesEmlab!B10</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
-      <c r="B21" t="str">
+    <row r="23" spans="2:9">
+      <c r="B23" t="str">
         <f>[1]TechnologiesEmlab!A11</f>
         <v>Lignite PSC</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <f>[1]TechnologiesEmlab!C11</f>
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <f>[1]TechnologiesEmlab!D11</f>
         <v>5</v>
       </c>
-      <c r="E21">
+      <c r="E23">
         <f>[1]TechnologiesEmlab!E11</f>
         <v>40</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <f>[1]TechnologiesEmlab!F11</f>
         <v>40</v>
       </c>
-      <c r="I21" t="str">
+      <c r="I23" t="str">
         <f>[1]TechnologiesEmlab!B11</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
-      <c r="B22" t="str">
+    <row r="24" spans="2:9">
+      <c r="B24" t="str">
         <f>[1]TechnologiesEmlab!A12</f>
         <v>Fuel oil PGT</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <f>[1]TechnologiesEmlab!C12</f>
         <v>1</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <f>[1]TechnologiesEmlab!D12</f>
         <v>1</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <f>[1]TechnologiesEmlab!E12</f>
         <v>25</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <f>[1]TechnologiesEmlab!F12</f>
         <v>25</v>
       </c>
-      <c r="I22" t="str">
+      <c r="I24" t="str">
         <f>[1]TechnologiesEmlab!B12</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
-      <c r="B23" t="str">
+    <row r="25" spans="2:9">
+      <c r="B25" t="str">
         <f>[1]TechnologiesEmlab!A13</f>
         <v>Lithium_ion_battery</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <f>[1]TechnologiesEmlab!C13</f>
         <v>0</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <f>[1]TechnologiesEmlab!D13</f>
         <v>1</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <f>[1]TechnologiesEmlab!E13</f>
         <v>20</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <f>[1]TechnologiesEmlab!F13</f>
         <v>20</v>
       </c>
-      <c r="I23" t="str">
+      <c r="I25" t="str">
         <f>[1]TechnologiesEmlab!B13</f>
         <v>StorageTrader</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
-      <c r="B24" t="str">
+    <row r="26" spans="2:9">
+      <c r="B26" t="str">
         <f>[1]TechnologiesEmlab!A14</f>
         <v>Pumped_hydro</v>
       </c>
-      <c r="C24">
+      <c r="C26">
         <f>[1]TechnologiesEmlab!C14</f>
         <v>3</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <f>[1]TechnologiesEmlab!D14</f>
         <v>4</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <f>[1]TechnologiesEmlab!E14</f>
         <v>100</v>
       </c>
-      <c r="F24">
+      <c r="F26">
         <f>[1]TechnologiesEmlab!F14</f>
         <v>100</v>
       </c>
-      <c r="I24" t="str">
+      <c r="I26" t="str">
         <f>[1]TechnologiesEmlab!B14</f>
         <v>StorageTrader</v>
       </c>
     </row>
-    <row r="25" spans="2:9">
-      <c r="B25" t="str">
+    <row r="27" spans="2:9">
+      <c r="B27" t="str">
         <f>[1]TechnologiesEmlab!A15</f>
         <v>WTG_offshore</v>
       </c>
-      <c r="C25">
+      <c r="C27">
         <f>[1]TechnologiesEmlab!C15</f>
         <v>1</v>
       </c>
-      <c r="D25">
+      <c r="D27">
         <f>[1]TechnologiesEmlab!D15</f>
         <v>2</v>
       </c>
-      <c r="E25">
+      <c r="E27">
         <f>[1]TechnologiesEmlab!E15</f>
         <v>30</v>
       </c>
-      <c r="F25">
+      <c r="F27">
         <f>[1]TechnologiesEmlab!F15</f>
         <v>30</v>
       </c>
-      <c r="I25" t="str">
+      <c r="I27" t="str">
         <f>[1]TechnologiesEmlab!B15</f>
         <v>VariableRenewableOperator</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
-      <c r="B26" t="str">
+    <row r="28" spans="2:9">
+      <c r="B28" t="str">
         <f>[1]TechnologiesEmlab!A16</f>
         <v>WTG_onshore</v>
       </c>
-      <c r="C26">
+      <c r="C28">
         <f>[1]TechnologiesEmlab!C16</f>
         <v>1</v>
       </c>
-      <c r="D26">
+      <c r="D28">
         <f>[1]TechnologiesEmlab!D16</f>
         <v>1</v>
       </c>
-      <c r="E26">
+      <c r="E28">
         <f>[1]TechnologiesEmlab!E16</f>
         <v>25</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <f>[1]TechnologiesEmlab!F16</f>
         <v>25</v>
       </c>
-      <c r="I26" t="str">
+      <c r="I28" t="str">
         <f>[1]TechnologiesEmlab!B16</f>
         <v>VariableRenewableOperator</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
-      <c r="B27" t="str">
+    <row r="29" spans="2:9">
+      <c r="B29" t="str">
         <f>[1]TechnologiesEmlab!A17</f>
         <v>PV_utility_systems</v>
       </c>
-      <c r="C27">
+      <c r="C29">
         <f>[1]TechnologiesEmlab!C17</f>
         <v>1</v>
       </c>
-      <c r="D27">
+      <c r="D29">
         <f>[1]TechnologiesEmlab!D17</f>
         <v>1</v>
       </c>
-      <c r="E27">
+      <c r="E29">
         <f>[1]TechnologiesEmlab!E17</f>
         <v>25</v>
       </c>
-      <c r="F27">
+      <c r="F29">
         <f>[1]TechnologiesEmlab!F17</f>
         <v>25</v>
       </c>
-      <c r="I27" t="str">
+      <c r="I29" t="str">
         <f>[1]TechnologiesEmlab!B17</f>
         <v>VariableRenewableOperator</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
-      <c r="B28" t="str">
+    <row r="30" spans="2:9">
+      <c r="B30" t="str">
         <f>[1]TechnologiesEmlab!A18</f>
-        <v>Hydropower_reservoir_medium</v>
-      </c>
-      <c r="C28">
+        <v>PV_residential</v>
+      </c>
+      <c r="C30">
         <f>[1]TechnologiesEmlab!C18</f>
-        <v>2</v>
-      </c>
-      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="D30">
         <f>[1]TechnologiesEmlab!D18</f>
-        <v>5</v>
-      </c>
-      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="E30">
         <f>[1]TechnologiesEmlab!E18</f>
-        <v>60</v>
-      </c>
-      <c r="F28">
+        <v>25</v>
+      </c>
+      <c r="F30">
         <f>[1]TechnologiesEmlab!F18</f>
-        <v>60</v>
-      </c>
-      <c r="I28" t="str">
+        <v>25</v>
+      </c>
+      <c r="I30" t="str">
         <f>[1]TechnologiesEmlab!B18</f>
         <v>VariableRenewableOperator</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
-      <c r="B29" t="str">
+    <row r="31" spans="2:9">
+      <c r="B31" t="str">
         <f>[1]TechnologiesEmlab!A19</f>
-        <v>hydrogen_turbine</v>
-      </c>
-      <c r="C29">
+        <v>Hydropower_reservoir_medium</v>
+      </c>
+      <c r="C31">
         <f>[1]TechnologiesEmlab!C19</f>
         <v>2</v>
       </c>
-      <c r="D29">
+      <c r="D31">
         <f>[1]TechnologiesEmlab!D19</f>
-        <v>2</v>
-      </c>
-      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="E31">
         <f>[1]TechnologiesEmlab!E19</f>
-        <v>30</v>
-      </c>
-      <c r="F29">
+        <v>60</v>
+      </c>
+      <c r="F31">
         <f>[1]TechnologiesEmlab!F19</f>
-        <v>30</v>
-      </c>
-      <c r="I29" t="str">
+        <v>60</v>
+      </c>
+      <c r="I31" t="str">
         <f>[1]TechnologiesEmlab!B19</f>
-        <v>ConventionalPlantOperator</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9">
-      <c r="B30" t="str">
+        <v>VariableRenewableOperator</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" t="str">
         <f>[1]TechnologiesEmlab!A20</f>
-        <v>hydrogen_CHP</v>
-      </c>
-      <c r="C30">
+        <v>hydrogen_turbine</v>
+      </c>
+      <c r="C32">
         <f>[1]TechnologiesEmlab!C20</f>
         <v>2</v>
       </c>
-      <c r="D30">
+      <c r="D32">
         <f>[1]TechnologiesEmlab!D20</f>
         <v>2</v>
       </c>
-      <c r="E30">
+      <c r="E32">
         <f>[1]TechnologiesEmlab!E20</f>
         <v>30</v>
       </c>
-      <c r="F30">
+      <c r="F32">
         <f>[1]TechnologiesEmlab!F20</f>
         <v>30</v>
       </c>
-      <c r="I30" t="str">
+      <c r="I32" t="str">
         <f>[1]TechnologiesEmlab!B20</f>
         <v>ConventionalPlantOperator</v>
       </c>
     </row>
-    <row r="31" spans="2:9">
-      <c r="B31" t="str">
-        <f>[1]TechnologiesEmlab!A21</f>
-        <v>hydrogen_combined_cycle</v>
-      </c>
-      <c r="C31">
-        <f>[1]TechnologiesEmlab!C21</f>
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <f>[1]TechnologiesEmlab!D21</f>
-        <v>2</v>
-      </c>
-      <c r="E31">
-        <f>[1]TechnologiesEmlab!E21</f>
-        <v>30</v>
-      </c>
-      <c r="F31">
-        <f>[1]TechnologiesEmlab!F21</f>
-        <v>30</v>
-      </c>
-      <c r="I31" t="str">
-        <f>[1]TechnologiesEmlab!B21</f>
-        <v>ConventionalPlantOperator</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" t="s">
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="3" t="s">
+    <row r="39" spans="1:11">
+      <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
-      <c r="B35" t="s">
+    <row r="40" spans="1:11">
+      <c r="B40" t="s">
         <v>6</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="D35">
+      <c r="D40">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
-      <c r="C36" t="s">
+    <row r="41" spans="1:11">
+      <c r="C41" t="s">
         <v>7</v>
       </c>
-      <c r="D36">
+      <c r="D41">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
-      <c r="A39" t="s">
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
-      <c r="B40" t="str">
+    <row r="45" spans="1:11">
+      <c r="B45" t="str">
         <f>[1]EnergyProducers!A1</f>
         <v>Name</v>
       </c>
-      <c r="C40" t="str">
+      <c r="C45" t="str">
         <f>[1]EnergyProducers!B1</f>
         <v>investorMarket</v>
       </c>
-      <c r="D40" t="str">
+      <c r="D45" t="str">
         <f>[1]EnergyProducers!C1</f>
         <v>priceMarkUp</v>
       </c>
-      <c r="E40" t="str">
+      <c r="E45" t="str">
         <f>[1]EnergyProducers!D1</f>
         <v>willingToInvest</v>
       </c>
-      <c r="F40" t="str">
+      <c r="F45" t="str">
         <f>[1]EnergyProducers!E1</f>
         <v>downpaymentFractionOfCash</v>
       </c>
-      <c r="G40" t="str">
+      <c r="G45" t="str">
         <f>[1]EnergyProducers!F1</f>
         <v>dismantlingRequiredOperatingProfit</v>
       </c>
-      <c r="H40" t="str">
+      <c r="H45" t="str">
         <f>[1]EnergyProducers!H1</f>
         <v>loanInterestRate</v>
       </c>
-      <c r="I40" t="str">
+      <c r="I45" t="str">
         <f>[1]EnergyProducers!I1</f>
         <v>equityInterestRate</v>
       </c>
-      <c r="J40" t="str">
+      <c r="J45" t="str">
         <f>[1]EnergyProducers!J1</f>
         <v>longTermContractPastTimeHorizon</v>
       </c>
-      <c r="K40" t="str">
+      <c r="K45" t="str">
         <f>[1]EnergyProducers!K1</f>
         <v>longTermContractMargin</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
-      <c r="B41" t="str">
+    <row r="46" spans="1:11">
+      <c r="B46" t="str">
         <f>[1]EnergyProducers!A3</f>
         <v>ProducerNL</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C46" t="str">
         <f>[1]EnergyProducers!B3</f>
         <v>DutchElectricitySpotMarket</v>
       </c>
-      <c r="D41">
+      <c r="D46">
         <f>[1]EnergyProducers!C3</f>
         <v>0</v>
       </c>
-      <c r="E41" t="b">
+      <c r="E46" t="b">
         <f>[1]EnergyProducers!D3</f>
         <v>1</v>
       </c>
-      <c r="F41">
+      <c r="F46">
         <f>[1]EnergyProducers!E3</f>
         <v>0.5</v>
       </c>
-      <c r="G41">
+      <c r="G46">
         <f>[1]EnergyProducers!F3</f>
         <v>0</v>
       </c>
-      <c r="H41">
+      <c r="H46">
         <f>[1]EnergyProducers!H3</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I41">
+      <c r="I46">
         <f>[1]EnergyProducers!I3</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J41">
+      <c r="J46">
         <f>[1]EnergyProducers!J3</f>
         <v>3</v>
       </c>
-      <c r="K41">
+      <c r="K46">
         <f>[1]EnergyProducers!K3</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
-      <c r="B45" t="str">
+    <row r="50" spans="1:8">
+      <c r="B50" t="str">
         <f>[1]ElectricitySpotMarkets!A1</f>
         <v>Name</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C50" t="str">
         <f>[1]ElectricitySpotMarkets!B1</f>
         <v>valueOfLostLoad</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
-      <c r="B46" t="str">
+    <row r="51" spans="1:8">
+      <c r="B51" t="str">
         <f>[1]ElectricitySpotMarkets!A3</f>
-        <v>DutchElectricitySpotMarket</v>
-      </c>
-      <c r="C46">
+        <v>ElectricitySpotMarketNL</v>
+      </c>
+      <c r="C51">
         <f>[1]ElectricitySpotMarkets!B3</f>
         <v>4000</v>
       </c>
     </row>
-    <row r="50" spans="2:8">
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="54" spans="2:8">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="2:8">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="2:8">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="2:8">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="2:8">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="2:8">
+    <row r="55" spans="1:8">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -6813,7 +6813,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="2:8">
+    <row r="60" spans="1:8">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -6822,7 +6822,7 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="2:8">
+    <row r="61" spans="1:8">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -6831,7 +6831,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="2:8">
+    <row r="62" spans="1:8">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -6840,7 +6840,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="2:8">
+    <row r="63" spans="1:8">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -6849,7 +6849,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="2:8">
+    <row r="64" spans="1:8">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -6908,30 +6908,45 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
     </row>
     <row r="71" spans="2:8">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
     </row>
     <row r="72" spans="2:8">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
     </row>
     <row r="73" spans="2:8">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
     </row>
     <row r="74" spans="2:8">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
     </row>
     <row r="75" spans="2:8">
       <c r="B75" s="1"/>
@@ -7004,6 +7019,36 @@
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="2:5">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="2:5">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+    </row>
+    <row r="89" spans="2:5">
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="2:5">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="2:5">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7018,42 +7063,42 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="41" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="41" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7070,7 +7115,7 @@
         <v>2050</v>
       </c>
       <c r="E1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -7115,7 +7160,7 @@
         <v>168</v>
       </c>
       <c r="E4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7146,7 +7191,7 @@
         <v>6.73</v>
       </c>
       <c r="E6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -7177,7 +7222,7 @@
         <v>32.83</v>
       </c>
       <c r="E8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -7222,7 +7267,7 @@
         <v>14.65</v>
       </c>
       <c r="E11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -7298,20 +7343,55 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="3:15">
-      <c r="C23" s="26"/>
-    </row>
-    <row r="25" spans="3:15">
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23">
+        <v>14.65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24">
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" t="s">
+        <v>204</v>
+      </c>
+      <c r="B25">
+        <v>35</v>
+      </c>
       <c r="L25" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="3:15">
+    <row r="26" spans="1:15">
       <c r="L26" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="3:15">
+    <row r="28" spans="1:15">
       <c r="M28" s="20">
         <v>2030</v>
       </c>
@@ -7322,7 +7402,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="29" spans="3:15">
+    <row r="29" spans="1:15">
       <c r="M29" s="20">
         <v>20.63</v>
       </c>
@@ -7333,7 +7413,7 @@
         <v>12.52</v>
       </c>
     </row>
-    <row r="30" spans="3:15">
+    <row r="30" spans="1:15">
       <c r="M30" s="28">
         <f>M29*3.6</f>
         <v>74.268000000000001</v>
@@ -7347,13 +7427,13 @@
         <v>45.072000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:15">
+    <row r="31" spans="1:15">
       <c r="J31" s="27"/>
       <c r="M31" s="20"/>
       <c r="N31" s="20"/>
       <c r="O31" s="20"/>
     </row>
-    <row r="32" spans="3:15">
+    <row r="32" spans="1:15">
       <c r="C32" s="26"/>
       <c r="J32" s="27"/>
       <c r="M32" s="20"/>
@@ -7420,29 +7500,29 @@
   <sheetPr>
     <tabColor rgb="FFFF0066"/>
   </sheetPr>
-  <dimension ref="A1:AH75"/>
+  <dimension ref="A1:AH88"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J49" sqref="J49"/>
+      <selection pane="topRight" activeCell="R69" sqref="R69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.90625" customWidth="1"/>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.08984375" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.90625" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.6328125" customWidth="1"/>
-    <col min="14" max="14" width="1.7265625" customWidth="1"/>
-    <col min="19" max="19" width="21.36328125" customWidth="1"/>
+    <col min="13" max="13" width="1.5703125" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -8244,55 +8324,54 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B50" s="6">
-        <v>2020</v>
-      </c>
-      <c r="C50" s="6">
-        <v>2030</v>
-      </c>
-      <c r="D50" s="6">
-        <v>2050</v>
+    <row r="49" spans="1:4">
+      <c r="A49" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B49" s="6">
+        <v>0</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23">
-        <v>108000</v>
+        <v>187</v>
+      </c>
+      <c r="B51" s="6">
+        <v>2020</v>
+      </c>
+      <c r="C51" s="6">
+        <v>2030</v>
+      </c>
+      <c r="D51" s="6">
+        <v>2050</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B52" s="23"/>
-      <c r="C52" s="23">
-        <v>50000</v>
-      </c>
-      <c r="D52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23">
+        <v>108000</v>
+      </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B53" s="23"/>
       <c r="C53" s="23">
-        <v>27800</v>
-      </c>
-      <c r="D53" s="23">
-        <v>26000</v>
-      </c>
+        <v>50000</v>
+      </c>
+      <c r="D53" s="23"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B54" s="23"/>
       <c r="C54" s="23">
@@ -8304,147 +8383,149 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B55" s="23"/>
       <c r="C55" s="23">
         <v>27800</v>
       </c>
-      <c r="D55" s="23"/>
+      <c r="D55" s="23">
+        <v>26000</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="6" t="s">
-        <v>182</v>
+        <v>29</v>
       </c>
       <c r="B56" s="23"/>
       <c r="C56" s="23">
-        <v>32000</v>
+        <v>27800</v>
       </c>
       <c r="D56" s="23"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="6" t="s">
-        <v>40</v>
+        <v>182</v>
       </c>
       <c r="B57" s="23"/>
       <c r="C57" s="23">
-        <v>1000</v>
-      </c>
-      <c r="D57" s="23">
-        <v>800</v>
-      </c>
+        <v>32000</v>
+      </c>
+      <c r="D57" s="23"/>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B58" s="23"/>
       <c r="C58" s="23">
-        <v>13450</v>
+        <v>1000</v>
       </c>
       <c r="D58" s="23">
-        <v>13425</v>
+        <v>800</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="23">
-        <v>14950</v>
+        <v>13450</v>
       </c>
       <c r="D59" s="23">
-        <v>14850</v>
+        <v>13425</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B60" s="23">
-        <v>111166.3</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B60" s="23"/>
       <c r="C60" s="23">
-        <v>100000</v>
-      </c>
-      <c r="D60" s="23"/>
+        <v>14950</v>
+      </c>
+      <c r="D60" s="23">
+        <v>14850</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" s="23"/>
+        <v>41</v>
+      </c>
+      <c r="B61" s="23">
+        <v>111166.3</v>
+      </c>
       <c r="C61" s="23">
-        <v>7745</v>
-      </c>
-      <c r="D61" s="23">
-        <v>7423</v>
-      </c>
+        <v>100000</v>
+      </c>
+      <c r="D61" s="23"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="6" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
+      <c r="C62" s="23">
+        <v>7745</v>
+      </c>
       <c r="D62" s="23">
-        <v>40000</v>
+        <v>7423</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="23"/>
       <c r="D63" s="23">
-        <v>30000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B64" s="23"/>
       <c r="C64" s="23"/>
       <c r="D64" s="23">
-        <v>11250</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B65" s="23"/>
       <c r="C65" s="23"/>
       <c r="D65" s="23">
-        <v>8700</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>11250</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B66" s="23"/>
       <c r="C66" s="23"/>
       <c r="D66" s="23">
+        <v>8700</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="23"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23">
         <v>7000</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="6" t="s">
+    <row r="68" spans="1:5">
+      <c r="A68" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B67" s="23">
-        <v>61528.160000000003</v>
-      </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="B68" s="23">
         <v>61528.160000000003</v>
@@ -8452,97 +8533,285 @@
       <c r="C68" s="23"/>
       <c r="D68" s="23"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="A69" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B69" s="23">
-        <v>8575</v>
+        <v>61528.160000000003</v>
       </c>
       <c r="C69" s="23"/>
       <c r="D69" s="23"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B70" s="23">
-        <v>16000</v>
+        <v>8575</v>
       </c>
       <c r="C70" s="23"/>
       <c r="D70" s="23"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="A71" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" s="23">
+        <v>16000</v>
+      </c>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B71" s="23"/>
-      <c r="C71" s="23">
-        <f>(C73+C72)/2</f>
-        <v>10300</v>
-      </c>
-      <c r="D71" s="23">
-        <f>(D73+D72)/2</f>
-        <v>9300</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="B72" s="23"/>
       <c r="C72" s="23">
-        <v>12300</v>
+        <f>(C74+C73)/2</f>
+        <v>10300</v>
       </c>
       <c r="D72" s="23">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <f>(D74+D73)/2</f>
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="6" t="s">
-        <v>44</v>
+        <v>183</v>
       </c>
       <c r="B73" s="23"/>
       <c r="C73" s="23">
-        <v>8300</v>
+        <v>12300</v>
       </c>
       <c r="D73" s="23">
-        <v>7600</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B74" s="23"/>
       <c r="C74" s="23">
-        <v>30500</v>
+        <v>8300</v>
       </c>
       <c r="D74" s="23">
-        <v>24700</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B75" s="23"/>
       <c r="C75" s="23">
+        <v>30500</v>
+      </c>
+      <c r="D75" s="23">
+        <v>24700</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B76" s="23"/>
+      <c r="C76" s="23">
         <v>14700</v>
       </c>
-      <c r="D75" s="23">
+      <c r="D76" s="23">
         <v>12900</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="B80" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B81" s="30">
+        <f>INDEX($B$3:$D$26,MATCH(A81,$A$3:$A$26,0),3)</f>
+        <v>1020000</v>
+      </c>
+      <c r="C81" s="6">
+        <f t="shared" ref="C81:C88" si="0">INDEX($B$30:$D$49,MATCH(A81,$A$30:$A$49,0),1)</f>
+        <v>1.8</v>
+      </c>
+      <c r="D81" s="6">
+        <f>INDEX($B$52:$D$76,MATCH(A81,$A$52:$A$76,0),3)</f>
+        <v>800</v>
+      </c>
+      <c r="E81" s="31">
+        <f t="shared" ref="E81:E88" si="1">INDEX($B$30:$D$49,MATCH(A81,$A$30:$A$49,0),2)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B82" s="30">
+        <f t="shared" ref="B82:B87" si="2">INDEX($B$3:$D$26,MATCH(A82,$A$3:$A$26,0),3)</f>
+        <v>1444000</v>
+      </c>
+      <c r="C82" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D82" s="6">
+        <f>INDEX($B$52:$D$76,MATCH(A82,$A$52:$A$76,0),3)</f>
+        <v>24700</v>
+      </c>
+      <c r="E82" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B83" s="30">
+        <f t="shared" si="2"/>
+        <v>350000</v>
+      </c>
+      <c r="C83" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D83" s="6">
+        <f>INDEX($B$52:$D$76,MATCH(A83,$A$52:$A$76,0),3)</f>
+        <v>7600</v>
+      </c>
+      <c r="E83" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B84" s="30">
+        <f t="shared" si="2"/>
+        <v>688000</v>
+      </c>
+      <c r="C84" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D84" s="6">
+        <f>INDEX($B$52:$D$76,MATCH(A84,$A$52:$A$76,0),3)</f>
+        <v>11000</v>
+      </c>
+      <c r="E84" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B85" s="30">
+        <f t="shared" si="2"/>
+        <v>1127000</v>
+      </c>
+      <c r="C85" s="6">
+        <f t="shared" si="0"/>
+        <v>1.35</v>
+      </c>
+      <c r="D85" s="6">
+        <f>INDEX($B$52:$D$76,MATCH(A85,$A$52:$A$76,0),3)</f>
+        <v>12900</v>
+      </c>
+      <c r="E85" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="30">
+        <v>2040000</v>
+      </c>
+      <c r="C86" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="D86" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E86" s="31">
+        <f t="shared" si="1"/>
+        <v>0.309</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" s="30">
+        <f t="shared" si="2"/>
+        <v>435000</v>
+      </c>
+      <c r="C87" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="D87" s="6">
+        <f>INDEX($B$52:$D$76,MATCH(A87,$A$52:$A$76,0),3)</f>
+        <v>8700</v>
+      </c>
+      <c r="E87" s="31">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B88" s="30">
+        <v>6000000</v>
+      </c>
+      <c r="C88" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D88" s="6">
+        <v>100000</v>
+      </c>
+      <c r="E88" s="31">
+        <f t="shared" si="1"/>
+        <v>0.28499999999999998</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
+  <conditionalFormatting sqref="A3:A26">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A30:A48">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A26">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51:A75">
+  <conditionalFormatting sqref="A52:A76">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8552,150 +8821,123 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0BDE63-C164-44DB-BCC1-F1906C1F98B7}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="53.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="str">
         <f>[1]LoadShedders!A1</f>
         <v>Name</v>
       </c>
-      <c r="B1" t="str">
-        <f>[1]LoadShedders!B1</f>
-        <v>VOLL</v>
-      </c>
-      <c r="C1" t="str">
-        <f>[1]LoadShedders!C1</f>
-        <v>TimeSeriesFile</v>
-      </c>
-      <c r="D1" t="str">
-        <f>[1]LoadShedders!D1</f>
-        <v>TimeSeriesFileFuture</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="D1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="str">
         <f>[1]LoadShedders!A2</f>
         <v>base</v>
       </c>
-      <c r="B2">
+      <c r="C2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2">
         <f>[1]LoadShedders!B2</f>
         <v>4000</v>
       </c>
-      <c r="C2" t="str">
-        <f>[1]LoadShedders!C2</f>
-        <v>amiris-config/data/load.csv</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="str">
         <f>[1]LoadShedders!A3</f>
         <v>high</v>
       </c>
-      <c r="B3">
+      <c r="C3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3">
         <f>[1]LoadShedders!B3</f>
         <v>1500</v>
       </c>
-      <c r="C3" t="str">
-        <f>[1]LoadShedders!C3</f>
-        <v>amiris-config/data/LS_high.csv</v>
+      <c r="E3" s="15">
+        <v>0.1</v>
       </c>
       <c r="F3">
         <f>[1]LoadShedders!F3</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="str">
         <f>[1]LoadShedders!A4</f>
         <v>mid</v>
       </c>
-      <c r="B4">
+      <c r="C4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4">
         <f>[1]LoadShedders!B4</f>
         <v>500</v>
       </c>
-      <c r="C4" t="str">
-        <f>[1]LoadShedders!C4</f>
-        <v>amiris-config/data/LS_mid.csv</v>
+      <c r="E4" s="15">
+        <v>0.05</v>
       </c>
       <c r="F4">
         <f>[1]LoadShedders!F4</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" t="str">
         <f>[1]LoadShedders!A5</f>
         <v>low</v>
       </c>
-      <c r="B5">
+      <c r="C5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5">
         <f>[1]LoadShedders!B5</f>
         <v>250</v>
       </c>
-      <c r="C5" t="str">
-        <f>[1]LoadShedders!C5</f>
-        <v>amiris-config/data/LS_low.csv</v>
+      <c r="E5" s="15">
+        <v>0.05</v>
       </c>
       <c r="F5">
         <f>[1]LoadShedders!F5</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="str">
         <f>[1]LoadShedders!A6</f>
         <v>hydrogen</v>
       </c>
-      <c r="B6">
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" s="26">
         <f>[1]LoadShedders!B6</f>
         <v>33.374000000000002</v>
       </c>
-      <c r="C6" t="str">
-        <f>[1]LoadShedders!C6</f>
-        <v>amiris-config/data/LS_hydrogen_high.csv</v>
-      </c>
-      <c r="D6" t="str">
-        <f>[1]LoadShedders!D6</f>
-        <v>amiris-config/data/LS_hydrogen.csv</v>
-      </c>
-      <c r="E6" s="15">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <f>[1]LoadShedders!A7</f>
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <f>[1]LoadShedders!B7</f>
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <f>[1]LoadShedders!C7</f>
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <f>[1]LoadShedders!D7</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="15">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -8705,13 +8947,19 @@
       <c r="C8" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="15">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="B9">
         <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>186</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -8727,12 +8975,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -8980,17 +9228,17 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="23.36328125" customWidth="1"/>
-    <col min="5" max="5" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="4.81640625" customWidth="1"/>
-    <col min="14" max="14" width="1.7265625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="4.85546875" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -9862,7 +10110,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -9897,7 +10145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -9926,7 +10174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="15">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -9961,7 +10209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="15">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>122</v>
       </c>
@@ -9993,7 +10241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="15">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -10022,7 +10270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -10051,7 +10299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -10080,7 +10328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -10112,7 +10360,7 @@
         <v>2294.0239999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15">
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -10144,7 +10392,7 @@
         <v>2294.0239999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15">
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -10176,7 +10424,7 @@
         <v>22940.240000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="15">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -10208,7 +10456,7 @@
         <v>22940.240000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="15">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>125</v>
       </c>
@@ -10240,7 +10488,7 @@
         <v>6882.0720000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -10272,7 +10520,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="15">
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -10304,7 +10552,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="15">
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>133</v>
       </c>
@@ -10348,7 +10596,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="15">
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>133</v>
       </c>
@@ -10389,7 +10637,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="15">
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -10433,7 +10681,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15">
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>133</v>
       </c>
@@ -10474,7 +10722,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15">
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>133</v>
       </c>
@@ -10509,7 +10757,7 @@
         <v>344.82641033966041</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15">
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -10544,7 +10792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15">
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>133</v>
       </c>
@@ -10588,7 +10836,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15">
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>133</v>
       </c>
@@ -10629,7 +10877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="15">
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -10673,7 +10921,7 @@
         <v>24.74</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="15">
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>133</v>
       </c>
@@ -10714,7 +10962,7 @@
         <v>23.93</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="15">
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>133</v>
       </c>
@@ -10758,7 +11006,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="15">
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>133</v>
       </c>
@@ -10799,7 +11047,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="15">
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>133</v>
       </c>
@@ -10840,7 +11088,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="15">
+    <row r="63" spans="1:13">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -10881,7 +11129,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="15">
+    <row r="64" spans="1:13">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -10925,7 +11173,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15">
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>133</v>
       </c>
@@ -10966,7 +11214,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="15">
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -11010,7 +11258,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="15">
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>133</v>
       </c>
@@ -11051,7 +11299,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="15">
+    <row r="68" spans="1:13">
       <c r="A68" t="s">
         <v>133</v>
       </c>
@@ -11080,7 +11328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="15">
+    <row r="69" spans="1:13">
       <c r="A69" t="s">
         <v>133</v>
       </c>
@@ -11112,7 +11360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="15">
+    <row r="70" spans="1:13">
       <c r="A70" t="s">
         <v>133</v>
       </c>
@@ -11144,7 +11392,7 @@
         <v>1773.915272638189</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="15">
+    <row r="71" spans="1:13">
       <c r="A71" t="s">
         <v>133</v>
       </c>
@@ -11176,7 +11424,7 @@
         <v>17739.15272638189</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="15">
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -11208,7 +11456,7 @@
         <v>5321.745817914566</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="15">
+    <row r="73" spans="1:13">
       <c r="A73" t="s">
         <v>133</v>
       </c>
@@ -11252,7 +11500,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="15">
+    <row r="74" spans="1:13">
       <c r="A74" t="s">
         <v>138</v>
       </c>
@@ -11475,17 +11723,17 @@
       <selection activeCell="AK16" sqref="AK16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="9" width="13.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" customWidth="1"/>
-    <col min="12" max="34" width="2.453125" customWidth="1"/>
-    <col min="35" max="35" width="4.08984375" customWidth="1"/>
-    <col min="36" max="39" width="2.453125" customWidth="1"/>
-    <col min="40" max="40" width="7.6328125" customWidth="1"/>
-    <col min="41" max="44" width="1.7265625" customWidth="1"/>
-    <col min="45" max="45" width="6.26953125" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="34" width="2.42578125" customWidth="1"/>
+    <col min="35" max="35" width="4.140625" customWidth="1"/>
+    <col min="36" max="39" width="2.42578125" customWidth="1"/>
+    <col min="40" max="40" width="7.5703125" customWidth="1"/>
+    <col min="41" max="44" width="1.7109375" customWidth="1"/>
+    <col min="45" max="45" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -12495,12 +12743,12 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
plotting changes and changing AMIRIS version to 13
</commit_message>
<xml_diff>
--- a/data/MostImportantData.xlsx
+++ b/data/MostImportantData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7210BC-9508-40C9-A5D9-DAF40C660788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246A9691-E051-4CCE-B932-68C42803761B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="738" activeTab="1" xr2:uid="{B8782AFC-8070-4987-A54E-8F4783B58729}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="738" activeTab="4" xr2:uid="{B8782AFC-8070-4987-A54E-8F4783B58729}"/>
   </bookViews>
   <sheets>
     <sheet name="Technology" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="285">
   <si>
     <t>ElectricitySportMarket</t>
   </si>
@@ -903,6 +903,105 @@
   <si>
     <t>EV + heat pump + household + commercial + industrial</t>
   </si>
+  <si>
+    <r>
+      <t>Load</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Type of flexibility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>EV, heat pump, household, commercial, industrial</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FFD13438"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Sheddable </t>
+  </si>
+  <si>
+    <t>35.0% </t>
+  </si>
+  <si>
+    <t>Hydrogen </t>
+  </si>
+  <si>
+    <t>45.6% </t>
+  </si>
+  <si>
+    <t>Industrial heat </t>
+  </si>
+  <si>
+    <t>Shiftable </t>
+  </si>
+  <si>
+    <t>13.2% </t>
+  </si>
+  <si>
+    <t>High LS</t>
+  </si>
+  <si>
+    <t>Medium LS</t>
+  </si>
+  <si>
+    <t>Low LS</t>
+  </si>
+  <si>
+    <t>1.55%</t>
+  </si>
+  <si>
+    <t>3.1%</t>
+  </si>
+  <si>
+    <t>VOLL (€/MWh)</t>
+  </si>
+  <si>
+    <r>
+      <t>Load share</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Type of load shedder</t>
+  </si>
 </sst>
 </file>
 
@@ -917,7 +1016,7 @@
     <numFmt numFmtId="167" formatCode="&quot;€&quot;\ #,##0"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1098,6 +1197,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FFD13438"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1149,7 +1274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1220,6 +1345,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1274,7 +1559,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1330,14 +1615,59 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Comma 2" xfId="1" xr:uid="{660B22D1-3511-451A-B770-8E4B2498B7FA}"/>
@@ -1490,7 +1820,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3369,7 +3699,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3407,7 +3737,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="402286687"/>
@@ -3469,7 +3799,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="749431311"/>
@@ -3521,7 +3851,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3558,7 +3888,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5695,7 +6025,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B6715E7F-A3EB-4473-8DA3-E3314F1ABE21}" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B6715E7F-A3EB-4473-8DA3-E3314F1ABE21}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -6141,15 +6471,15 @@
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -7285,56 +7615,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3632514B-ABC6-4169-8B9E-B369CFE6C343}">
   <dimension ref="A2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="10" max="10" width="29.21875" customWidth="1"/>
-    <col min="11" max="11" width="67.77734375" customWidth="1"/>
-    <col min="12" max="12" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" customWidth="1"/>
+    <col min="11" max="11" width="67.7109375" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="23.4">
+    <row r="2" spans="1:13" ht="23.25">
       <c r="A2" s="6" t="s">
         <v>225</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37" t="s">
+      <c r="D2" s="40"/>
+      <c r="E2" s="40" t="s">
         <v>220</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
       <c r="H2" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="K2" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="39" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="31.2" customHeight="1">
+    <row r="3" spans="1:13" ht="31.15" customHeight="1">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -7359,20 +7689,20 @@
       <c r="H3" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="L3" s="39" t="s">
+      <c r="L3" s="38" t="s">
         <v>242</v>
       </c>
       <c r="M3">
         <v>0.45635560706442235</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="31.2" customHeight="1">
+    <row r="4" spans="1:13" ht="31.15" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>226</v>
       </c>
@@ -7397,20 +7727,20 @@
       <c r="H4" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="K4" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="38" t="s">
         <v>245</v>
       </c>
       <c r="M4">
         <v>0.1322461625216583</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="31.2" customHeight="1">
+    <row r="5" spans="1:13" ht="31.15" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>228</v>
       </c>
@@ -7435,20 +7765,20 @@
       <c r="H5" s="6">
         <v>40</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="38" t="s">
         <v>265</v>
       </c>
       <c r="M5">
         <v>4.307958095190436E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="31.2" customHeight="1">
+    <row r="6" spans="1:13" ht="31.15" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>227</v>
       </c>
@@ -7473,20 +7803,20 @@
       <c r="H6" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="K6" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="38" t="s">
         <v>265</v>
       </c>
       <c r="M6">
         <v>6.1060639474064503E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="31.2" customHeight="1">
+    <row r="7" spans="1:13" ht="31.15" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>221</v>
       </c>
@@ -7511,13 +7841,13 @@
       <c r="H7" s="6">
         <v>1</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="K7" s="40" t="s">
+      <c r="K7" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="38" t="s">
         <v>265</v>
       </c>
       <c r="M7">
@@ -7525,7 +7855,7 @@
         <v>0.6927419900120495</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="31.2" customHeight="1">
+    <row r="8" spans="1:13" ht="31.15" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>216</v>
       </c>
@@ -7551,7 +7881,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="31.2" customHeight="1">
+    <row r="9" spans="1:13" ht="31.15" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>232</v>
       </c>
@@ -7627,24 +7957,24 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="D15" s="38"/>
+      <c r="D15" s="37"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="D16" s="38"/>
+      <c r="D16" s="37"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="D17" s="38"/>
+      <c r="D17" s="37"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="36"/>
-      <c r="D18" s="38"/>
+      <c r="D18" s="37"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="36"/>
-      <c r="D19" s="38"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="D20" s="38"/>
+      <c r="D20" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7668,38 +7998,38 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="38" max="41" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="41" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8108,22 +8438,22 @@
       <selection pane="topRight" activeCell="R69" sqref="R69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.5546875" customWidth="1"/>
-    <col min="14" max="14" width="1.6640625" customWidth="1"/>
-    <col min="19" max="19" width="21.44140625" customWidth="1"/>
+    <col min="13" max="13" width="1.5703125" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -9422,19 +9752,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0BDE63-C164-44DB-BCC1-F1906C1F98B7}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="3.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -9563,8 +9893,116 @@
         <v>0.3</v>
       </c>
     </row>
+    <row r="14" spans="1:7" ht="26.25" thickBot="1">
+      <c r="C14" s="46" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
+      <c r="C15" s="49" t="s">
+        <v>269</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>281</v>
+      </c>
+      <c r="G15" s="45">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1">
+      <c r="C16" s="50"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="G16" s="45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="35.25" customHeight="1" thickBot="1">
+      <c r="C17" s="50"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="G17" s="45">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="15.75" thickBot="1">
+      <c r="C18" s="51"/>
+      <c r="D18" s="41" t="s">
+        <v>263</v>
+      </c>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41" t="s">
+        <v>271</v>
+      </c>
+      <c r="G18" s="45">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" ht="15.75" thickBot="1">
+      <c r="C19" s="52" t="s">
+        <v>272</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="G19" s="45">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20" s="53" t="s">
+        <v>274</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>275</v>
+      </c>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="G20" s="55">
+        <v>4000</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9576,12 +10014,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -9829,17 +10267,17 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="4.88671875" customWidth="1"/>
-    <col min="14" max="14" width="1.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="4.85546875" customWidth="1"/>
+    <col min="14" max="14" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -10711,7 +11149,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" ht="15.75">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -10746,7 +11184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" ht="15.75">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -10775,7 +11213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" ht="15.75">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -10810,7 +11248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" ht="15.75">
       <c r="A39" t="s">
         <v>122</v>
       </c>
@@ -10842,7 +11280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" ht="15.75">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -10871,7 +11309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" ht="15.75">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -10900,7 +11338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" ht="15.75">
       <c r="A42" t="s">
         <v>122</v>
       </c>
@@ -10929,7 +11367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" ht="15.75">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -10961,7 +11399,7 @@
         <v>2294.0239999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" ht="15.75">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -10993,7 +11431,7 @@
         <v>2294.0239999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" ht="15.75">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -11025,7 +11463,7 @@
         <v>22940.240000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" ht="15.75">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -11057,7 +11495,7 @@
         <v>22940.240000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" ht="15.75">
       <c r="A47" t="s">
         <v>125</v>
       </c>
@@ -11089,7 +11527,7 @@
         <v>6882.0720000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" ht="15.75">
       <c r="A48" t="s">
         <v>133</v>
       </c>
@@ -11121,7 +11559,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" ht="15.75">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -11153,7 +11591,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" ht="15.75">
       <c r="A50" t="s">
         <v>133</v>
       </c>
@@ -11197,7 +11635,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" ht="15.75">
       <c r="A51" t="s">
         <v>133</v>
       </c>
@@ -11238,7 +11676,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" ht="15.75">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -11282,7 +11720,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" ht="15.75">
       <c r="A53" t="s">
         <v>133</v>
       </c>
@@ -11323,7 +11761,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" ht="15.75">
       <c r="A54" t="s">
         <v>133</v>
       </c>
@@ -11358,7 +11796,7 @@
         <v>344.82641033966041</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" ht="15.75">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -11393,7 +11831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" ht="15.75">
       <c r="A56" t="s">
         <v>133</v>
       </c>
@@ -11437,7 +11875,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" ht="15.75">
       <c r="A57" t="s">
         <v>133</v>
       </c>
@@ -11478,7 +11916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" ht="15.75">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -11522,7 +11960,7 @@
         <v>24.74</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" ht="15.75">
       <c r="A59" t="s">
         <v>133</v>
       </c>
@@ -11563,7 +12001,7 @@
         <v>23.93</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" ht="15.75">
       <c r="A60" t="s">
         <v>133</v>
       </c>
@@ -11607,7 +12045,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" ht="15.75">
       <c r="A61" t="s">
         <v>133</v>
       </c>
@@ -11648,7 +12086,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" ht="15.75">
       <c r="A62" t="s">
         <v>133</v>
       </c>
@@ -11689,7 +12127,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" ht="15.75">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -11730,7 +12168,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" ht="15.75">
       <c r="A64" t="s">
         <v>133</v>
       </c>
@@ -11774,7 +12212,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" ht="15.75">
       <c r="A65" t="s">
         <v>133</v>
       </c>
@@ -11815,7 +12253,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" ht="15.75">
       <c r="A66" t="s">
         <v>133</v>
       </c>
@@ -11859,7 +12297,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" ht="15.75">
       <c r="A67" t="s">
         <v>133</v>
       </c>
@@ -11900,7 +12338,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" ht="15.75">
       <c r="A68" t="s">
         <v>133</v>
       </c>
@@ -11929,7 +12367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" ht="15.75">
       <c r="A69" t="s">
         <v>133</v>
       </c>
@@ -11961,7 +12399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" ht="15.75">
       <c r="A70" t="s">
         <v>133</v>
       </c>
@@ -11993,7 +12431,7 @@
         <v>1773.915272638189</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" ht="15.75">
       <c r="A71" t="s">
         <v>133</v>
       </c>
@@ -12025,7 +12463,7 @@
         <v>17739.15272638189</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" ht="15.75">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -12057,7 +12495,7 @@
         <v>5321.745817914566</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" ht="15.75">
       <c r="A73" t="s">
         <v>133</v>
       </c>
@@ -12101,7 +12539,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" ht="15.75">
       <c r="A74" t="s">
         <v>138</v>
       </c>
@@ -12324,17 +12762,17 @@
       <selection activeCell="AK16" sqref="AK16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="9" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" customWidth="1"/>
-    <col min="12" max="34" width="2.44140625" customWidth="1"/>
-    <col min="35" max="35" width="4.109375" customWidth="1"/>
-    <col min="36" max="39" width="2.44140625" customWidth="1"/>
-    <col min="40" max="40" width="7.5546875" customWidth="1"/>
-    <col min="41" max="44" width="1.6640625" customWidth="1"/>
-    <col min="45" max="45" width="6.33203125" customWidth="1"/>
+    <col min="8" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" customWidth="1"/>
+    <col min="12" max="34" width="2.42578125" customWidth="1"/>
+    <col min="35" max="35" width="4.140625" customWidth="1"/>
+    <col min="36" max="39" width="2.42578125" customWidth="1"/>
+    <col min="40" max="40" width="7.5703125" customWidth="1"/>
+    <col min="41" max="44" width="1.7109375" customWidth="1"/>
+    <col min="45" max="45" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -13344,12 +13782,12 @@
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>